<commit_message>
Updated entities in the database schema.
</commit_message>
<xml_diff>
--- a/documents/테이블 정의서.xlsx
+++ b/documents/테이블 정의서.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26712"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\siat_final_project\TJSManager\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE7A6BC9-B630-4A51-974A-B7E445BB0F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1F3C665-1A6D-44B3-B702-49B0E94C8F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" firstSheet="13" activeTab="13" xr2:uid="{23F431DE-E5DE-4A76-B807-59BB60D14234}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" firstSheet="8" activeTab="8" xr2:uid="{23F431DE-E5DE-4A76-B807-59BB60D14234}"/>
   </bookViews>
   <sheets>
     <sheet name="멤버쉽 고객 구매 이력" sheetId="10" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="물품별 구매자 기록" sheetId="8" r:id="rId3"/>
     <sheet name="판매 이력" sheetId="5" r:id="rId4"/>
     <sheet name="입고 신청 이력" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="14" r:id="rId6"/>
+    <sheet name="승인대기 입고 신청 이력" sheetId="14" r:id="rId6"/>
     <sheet name="재고 현황" sheetId="3" r:id="rId7"/>
     <sheet name="모든 상품 기본 정보" sheetId="2" r:id="rId8"/>
     <sheet name="직원 근무 기록" sheetId="7" r:id="rId9"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="230">
   <si>
     <t>테이블정의서</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -143,8 +143,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>FOREIGN KEY SALES_RECORD( SALES_NUM )</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>PRIMARY KEY, FOREIGN KEY SALES_RECORD( SALES_NUM )</t>
   </si>
   <si>
     <t>* 판매 번호를 통해 해당 판매 정보 조회 가능</t>
@@ -440,381 +439,387 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>APPROVED_DATE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>점장 승인 일</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 승인하지 않았으면 NULL, 승인하면 승인한 날짜 저장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM_STOCK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item_stock</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY KEY,
+FOREIGN KEY ITEM_INFO(ITEM_NUM)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY KEY,
+FOREIGN KEY MANAGED_STORE( STORE_NUM )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN_CNT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고량</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT_CNT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>출고량</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DROP_CNT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>미판매량</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 유통기한이 지났거나 분실 등의 이유로 판매하지 못한 상품의 개수</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>진열 위치</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 어떠한 이유로 진열할 수 없는 경우도 존재</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SALE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>할인율</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER(2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 할인을 안 하는 경우에는 0으로 표시</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EVENT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>행사 여부</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 행사 이름을 문자열 그대로 저장("1+1", "2+1" 등)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM_INFO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item_info</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>item_name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품명</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(100)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품 분류</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(60)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONSUMER_PRICE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>소비자판매가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRODUCT_DATE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>제조일자</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXPIRATION_DATE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>유통기한</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 유통기한이 없는 제품도 존재</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMPLOYEE_WORK_LOG</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HRM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Employee_work_log</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>WORK_LOG_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무 일지 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMP_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>소속 지점 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>START_WORK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>출근 시각</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>END_WORK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>퇴근 시각</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DISCRIPTION</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무 상태</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 특별한 일 없이 출퇴근 했다면 "근무"
+* 연·월차 / 반차 사용 시 "휴가"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMPLOYEE_PAY_RECORD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Employee_pay_record</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECORD_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기록 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAY_DATE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>급여 지급일</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAY_VALUE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지급 금액</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMPLOYEE_INFO_UPDATED</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Employee_info_updated</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPDATE_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정 기록 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정 대상의 직원 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정 대상 소속 지점 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPDATED_DATE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정일</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPDATER_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정한 직원 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPDATER_STORE_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정한 직원 소속 지점 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMPLOYEE_PERFORMANCE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Employee_performance</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PERFORMANCE_NUM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사 평가 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사 평가 대상 직원 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOREIGN KEY MANAGED_STORE( STORE_NUN )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사 평가 작성자 번호(직원 번호)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원은 작성 불가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>WRITER_STORE_NUM</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>신청서 작성자 소속 지점 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>APPROVED_DATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>점장 승인 일</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 승인하지 않았으면 NULL, 승인하면 승인한 날짜 저장</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ITEM_STOCK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item_stock</t>
+    <t>인사 평가 작성자 소속 지점 번호</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATED_DATE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성일</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TYPE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>평가 분류</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* "주간" / "월간" / "연간"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>평가 내용</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(6000)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 한글(3바이트) 기준으로 2000자까지 작성 가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Employee</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PRIMARY KEY,
 FOREIGN KEY( STORE_NUM )</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>IN_CNT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>입고량</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>OUT_CNT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>출고량</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DROP_CNT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>미판매량</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 유통기한이 지났거나 분실 등의 이유로 판매하지 못한 상품의 개수</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>진열 위치</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 어떠한 이유로 진열할 수 없는 경우도 존재</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SALE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>할인율</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>NUMBER(2)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 할인을 안 하는 경우에는 0으로 표시</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EVENT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>행사 여부</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 행사 이름을 문자열 그대로 저장("1+1", "2+1" 등)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ITEM_INFO</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item_info</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>item_name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>물품명</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(100)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>물품 분류</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(60)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CONSUMER_PRICE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>소비자판매가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRODUCT_DATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>제조일자</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXPIRATION_DATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유통기한</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 유통기한이 없는 제품도 존재</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMPLOYEE_WORK_LOG</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>HRM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Employee_work_log</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>WORK_LOG_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>근무 일지 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMP_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>직원 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>소속 지점 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>START_WORK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>출근 시각</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>END_WORK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>퇴근 시각</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DISCRIPTION</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>근무 상태</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 특별한 일 없이 출퇴근 했다면 "근무"
-* 연·월차 / 반차 사용 시 "휴가"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMPLOYEE_PAY_RECORD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Employee_pay_record</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>RECORD_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>기록 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAY_DATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>급여 지급일</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAY_VALUE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>지급 금액</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMPLOYEE_INFO_UPDATED</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Employee_info_updated</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPDATE_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정 기록 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정 대상의 직원 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정 대상 소속 지점 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPDATED_DATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정일</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPDATER_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정한 직원 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>UPDATER_STORE_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정한 직원 소속 지점 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMPLOYEE_PERFORMANCE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Employee_performance</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PERFORMANCE_NUM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>인사 평가 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>인사 평가 대상 직원 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>FOREIGN KEY MANAGED_STORE( STORE_NUN )</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>인사 평가 작성자 번호(직원 번호)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 일반 직원은 작성 불가능</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>인사 평가 작성자 소속 지점 번호</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CREATED_DATE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성일</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TYPE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>평가 분류</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* "주간" / "월간" / "연간"</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>평가 내용</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(6000)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 한글(3바이트) 기준으로 2000자까지 작성 가능</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>employee</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Employee</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -1421,12 +1426,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1446,6 +1445,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1469,6 +1474,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1484,6 +1498,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1492,21 +1512,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1825,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5BA791-22E2-45EB-9919-50DE9D7B91D9}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -1870,58 +1875,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -1942,12 +1947,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="119.45" thickTop="1">
       <c r="A8" s="4">
@@ -1968,12 +1973,12 @@
       <c r="F8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" ht="79.150000000000006">
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" ht="105.6">
       <c r="A9" s="7">
         <f>SUM(A8,1)</f>
         <v>2</v>
@@ -1993,12 +1998,12 @@
       <c r="F9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="24"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" ht="26.45">
       <c r="A10" s="7">
@@ -2018,12 +2023,12 @@
         <v>20</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="26.45">
       <c r="A11" s="7">
@@ -2454,11 +2459,6 @@
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="G7:J7"/>
@@ -2474,14 +2474,19 @@
     <mergeCell ref="G25:J25"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G28:J28"/>
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G16:J16"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G28:J28"/>
     <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
     <mergeCell ref="G35:J35"/>
     <mergeCell ref="G36:J36"/>
     <mergeCell ref="G37:J37"/>
@@ -2498,7 +2503,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -2542,58 +2547,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="21"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2614,22 +2619,22 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>156</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>19</v>
@@ -2640,10 +2645,10 @@
       <c r="F8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="53.45" thickTop="1">
       <c r="A9" s="7">
@@ -2651,10 +2656,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -2665,10 +2670,10 @@
       <c r="F9" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="79.150000000000006">
       <c r="A10" s="7">
@@ -2679,7 +2684,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>19</v>
@@ -2701,10 +2706,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>40</v>
@@ -2724,10 +2729,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>19</v>
@@ -2736,10 +2741,10 @@
         <v>20</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="7">
@@ -3198,7 +3203,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -3242,58 +3247,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="21"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -3314,22 +3319,22 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>164</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>19</v>
@@ -3340,10 +3345,10 @@
       <c r="F8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="53.45" thickTop="1">
       <c r="A9" s="7">
@@ -3351,10 +3356,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -3365,10 +3370,10 @@
       <c r="F9" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="24"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" ht="79.150000000000006">
       <c r="A10" s="7">
@@ -3379,7 +3384,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>19</v>
@@ -3401,10 +3406,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>40</v>
@@ -3424,10 +3429,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>170</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>19</v>
@@ -3438,10 +3443,10 @@
       <c r="F12" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:10" ht="79.150000000000006">
       <c r="A13" s="7">
@@ -3449,10 +3454,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>19</v>
@@ -3910,7 +3915,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -3954,58 +3959,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="21"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -4026,22 +4031,22 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27.6" thickTop="1" thickBot="1">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>19</v>
@@ -4052,10 +4057,10 @@
       <c r="F8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="46"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:10" ht="53.45" thickTop="1">
       <c r="A9" s="7">
@@ -4063,10 +4068,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -4077,10 +4082,10 @@
       <c r="F9" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
     </row>
     <row r="10" spans="1:10" ht="79.900000000000006" thickBot="1">
       <c r="A10" s="7">
@@ -4091,7 +4096,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>19</v>
@@ -4100,7 +4105,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G10" s="31"/>
       <c r="H10" s="32"/>
@@ -4116,7 +4121,7 @@
         <v>95</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>19</v>
@@ -4127,12 +4132,12 @@
       <c r="F11" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="44"/>
+      <c r="G11" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="36"/>
     </row>
     <row r="12" spans="1:10" ht="79.150000000000006">
       <c r="A12" s="7">
@@ -4140,7 +4145,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>181</v>
@@ -4152,7 +4157,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="32"/>
@@ -4177,10 +4182,10 @@
         <v>20</v>
       </c>
       <c r="F13" s="13"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:10" ht="26.45">
       <c r="A14" s="7">
@@ -4200,12 +4205,12 @@
         <v>20</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="15" spans="1:10" ht="26.45">
       <c r="A15" s="7">
@@ -4213,7 +4218,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>187</v>
@@ -4600,14 +4605,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
     <mergeCell ref="G31:J31"/>
     <mergeCell ref="G25:J25"/>
     <mergeCell ref="G15:J15"/>
@@ -4615,6 +4612,12 @@
     <mergeCell ref="G17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="G24:J24"/>
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="G33:J33"/>
@@ -4622,29 +4625,31 @@
     <mergeCell ref="G35:J35"/>
     <mergeCell ref="G36:J36"/>
     <mergeCell ref="G37:J37"/>
-    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="G19:J19"/>
     <mergeCell ref="G20:J20"/>
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G9:J9"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G24:J24"/>
     <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B1:I2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="B1:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4656,7 +4661,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -4700,58 +4705,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>190</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="21"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>191</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -4772,22 +4777,22 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" customHeight="1" thickTop="1">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>19</v>
@@ -4796,12 +4801,12 @@
         <v>20</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+        <v>192</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="79.150000000000006">
       <c r="A9" s="7">
@@ -4812,7 +4817,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -4821,7 +4826,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="32"/>
@@ -4834,20 +4839,20 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
@@ -4859,10 +4864,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>37</v>
@@ -4871,10 +4876,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" ht="26.45">
       <c r="A12" s="7">
@@ -4882,10 +4887,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>37</v>
@@ -4895,7 +4900,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -4907,10 +4912,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>43</v>
@@ -4920,7 +4925,7 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -4932,10 +4937,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>40</v>
@@ -4955,10 +4960,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>47</v>
@@ -4968,7 +4973,7 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -4980,10 +4985,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>40</v>
@@ -5003,10 +5008,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>19</v>
@@ -5016,7 +5021,7 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
@@ -5028,10 +5033,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>19</v>
@@ -5041,7 +5046,7 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
@@ -5401,8 +5406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141A7512-D431-462C-A6A3-3DDF3FE6DA10}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -5446,58 +5451,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="J4" s="21"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="1:10" ht="16.5">
-      <c r="A6" s="20" t="s">
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -5518,12 +5523,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" thickTop="1">
       <c r="A8" s="4">
@@ -5544,10 +5549,10 @@
       <c r="F8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="39.6">
       <c r="A9" s="7">
@@ -5555,20 +5560,20 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -5580,10 +5585,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>37</v>
@@ -5592,12 +5597,12 @@
         <v>20</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="G10" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="26.45">
       <c r="A11" s="7">
@@ -5605,10 +5610,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>37</v>
@@ -5618,7 +5623,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -5630,10 +5635,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>43</v>
@@ -5643,7 +5648,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -6082,7 +6087,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -6126,58 +6131,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -6198,12 +6203,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" thickTop="1">
       <c r="A8" s="4">
@@ -6224,10 +6229,10 @@
       <c r="F8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="26.45">
       <c r="A9" s="7">
@@ -6269,10 +6274,10 @@
         <v>20</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="26.45">
       <c r="A11" s="7">
@@ -6777,7 +6782,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -6821,58 +6826,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -6893,12 +6898,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="106.15" thickTop="1">
       <c r="A8" s="4">
@@ -6919,10 +6924,10 @@
       <c r="F8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="26.45">
       <c r="A9" s="7">
@@ -6966,12 +6971,12 @@
         <v>20</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="7">
@@ -7435,8 +7440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB0DFE-D17B-4A38-A801-C4E0875195B3}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -7480,58 +7485,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>66</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -7552,12 +7557,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" thickTop="1">
       <c r="A8" s="4">
@@ -7578,10 +7583,10 @@
       <c r="F8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="79.150000000000006">
       <c r="A9" s="7">
@@ -7650,10 +7655,10 @@
       <c r="F11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="7">
@@ -8131,7 +8136,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -8175,58 +8180,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>81</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>82</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -8247,12 +8252,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" thickTop="1">
       <c r="A8" s="4">
@@ -8273,10 +8278,10 @@
       <c r="F8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="79.150000000000006">
       <c r="A9" s="7">
@@ -8346,10 +8351,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" ht="26.45">
       <c r="A12" s="7">
@@ -8818,8 +8823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B5E0EE-7609-48D5-9869-8C09933E2466}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -8863,58 +8868,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
         <v>91</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
         <v>92</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -8935,12 +8940,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" thickTop="1">
       <c r="A8" s="4">
@@ -8961,10 +8966,10 @@
       <c r="F8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="79.150000000000006">
       <c r="A9" s="7">
@@ -9034,10 +9039,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" ht="26.45">
       <c r="A12" s="7">
@@ -9087,7 +9092,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:10" ht="39.6">
+    <row r="14" spans="1:10" ht="41.25" customHeight="1">
       <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -9099,43 +9104,33 @@
         <v>99</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
+      </c>
+      <c r="E14" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="1:10" ht="26.45">
+    <row r="15" spans="1:10">
       <c r="A15" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(A14,1)</f>
         <v>8</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="7">
@@ -9536,8 +9531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C2582E-94D0-4600-B70F-7DA48EDBD766}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -9581,58 +9576,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -9653,12 +9648,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" customHeight="1" thickTop="1">
       <c r="A8" s="4">
@@ -9677,14 +9672,14 @@
         <v>20</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
-    </row>
-    <row r="9" spans="1:10" ht="79.150000000000006">
+        <v>103</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:10" ht="105.6">
       <c r="A9" s="7">
         <f>SUM(A8,1)</f>
         <v>2</v>
@@ -9702,7 +9697,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="32"/>
@@ -9715,10 +9710,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>19</v>
@@ -9738,10 +9733,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>19</v>
@@ -9750,10 +9745,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="7">
@@ -9761,10 +9756,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>19</v>
@@ -9774,7 +9769,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -9786,10 +9781,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>47</v>
@@ -9799,7 +9794,7 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -9811,20 +9806,20 @@
         <v>7</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
@@ -9836,10 +9831,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>37</v>
@@ -9849,7 +9844,7 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -10254,11 +10249,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE51EB42-2843-4137-B03D-4B7C06449F1E}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
+  <cols>
+    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.45" customHeight="1">
       <c r="A1" s="1"/>
@@ -10299,58 +10296,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -10371,12 +10368,12 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" thickTop="1">
       <c r="A8" s="4">
@@ -10397,10 +10394,10 @@
       <c r="F8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="26.45">
       <c r="A9" s="7">
@@ -10408,13 +10405,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>20</v>
@@ -10431,22 +10428,22 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="26.45">
       <c r="A11" s="7">
@@ -10454,10 +10451,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>19</v>
@@ -10477,10 +10474,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>40</v>
@@ -10500,10 +10497,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>40</v>
@@ -10513,7 +10510,7 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -10936,8 +10933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDEE289-220A-4760-93F2-E3C5BFA6119F}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -10981,58 +10978,58 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="5" spans="1:10" ht="16.5">
+      <c r="A5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="27" t="s">
         <v>139</v>
-      </c>
-      <c r="J4" s="21"/>
-    </row>
-    <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="27" t="s">
-        <v>140</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -11053,22 +11050,22 @@
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="27" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>19</v>
@@ -11079,10 +11076,10 @@
       <c r="F8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="53.45" thickTop="1">
       <c r="A9" s="7">
@@ -11090,10 +11087,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -11104,10 +11101,10 @@
       <c r="F9" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="79.150000000000006">
       <c r="A10" s="7">
@@ -11118,7 +11115,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>19</v>
@@ -11140,15 +11137,17 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="31"/>
       <c r="H11" s="32"/>
@@ -11161,20 +11160,22 @@
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:10" ht="26.45">
       <c r="A13" s="7">
@@ -11182,10 +11183,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>47</v>
@@ -11195,7 +11196,7 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>

</xml_diff>